<commit_message>
n2adr filter board and jumper build8
</commit_message>
<xml_diff>
--- a/hardware/hl/bom/bom.assembly.xlsx
+++ b/hardware/hl/bom/bom.assembly.xlsx
@@ -50,7 +50,7 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Part Reference Link</t>
+    <t xml:space="preserve">Part Supplier and Reference Links</t>
   </si>
   <si>
     <t xml:space="preserve">0.1uF 0603&gt;=X5R&gt;=25V&lt;=20%</t>
@@ -423,7 +423,7 @@
   </si>
   <si>
     <t xml:space="preserve">EC2-3NU
-NA-3W-K</t>
+EC2-3NJ</t>
   </si>
   <si>
     <t xml:space="preserve">K2</t>
@@ -951,10 +951,10 @@
     <t xml:space="preserve">U19</t>
   </si>
   <si>
-    <t xml:space="preserve">21cm PFTE 24to30AWG wire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30AWG Teflon PFTE</t>
+    <t xml:space="preserve">21cm PFTE silver plated 24to30AWG wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400R0111-24-9</t>
   </si>
   <si>
     <t xml:space="preserve">W1</t>
@@ -1020,7 +1020,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1044,6 +1044,12 @@
     <font>
       <b val="true"/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1090,7 +1096,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1103,12 +1109,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1128,25 +1142,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G85"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0102040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.780612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.18367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="73.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1122448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.24489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="58.4948979591837"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="53.0714285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.9183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="50.1989795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="50.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,7 +1186,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1180,6 +1198,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="248.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1191,16 +1213,16 @@
       <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -1213,6 +1235,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0603C104M5RACTU")</f>
         <v>http://www.octopart.com/search?q=C0603C104M5RACTU</v>
       </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C1608X7R1E104K080AA")</f>
+        <v>http://www.octopart.com/search?q=C1608X7R1E104K080AA</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1224,16 +1250,16 @@
       <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -1246,6 +1272,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM188R60J106KE47D")</f>
         <v>http://www.octopart.com/search?q=GRM188R60J106KE47D</v>
       </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM188R60J106ME47D")</f>
+        <v>http://www.octopart.com/search?q=GRM188R60J106ME47D</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1266,7 +1296,7 @@
       <c r="F4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="H4" s="0" t="n">
@@ -1290,7 +1320,7 @@
       <c r="C5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -1299,7 +1329,7 @@
       <c r="F5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -1312,6 +1342,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL10B472KB8NNNC")</f>
         <v>http://www.octopart.com/search?q=CL10B472KB8NNNC</v>
       </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0603C472K5RACTU")</f>
+        <v>http://www.octopart.com/search?q=C0603C472K5RACTU</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1323,16 +1357,16 @@
       <c r="C6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H6" s="0" t="n">
@@ -1345,6 +1379,22 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21A226MOCLRNC")</f>
         <v>http://www.octopart.com/search?q=CL21A226MOCLRNC</v>
       </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM21BR61E226ME44L")</f>
+        <v>http://www.octopart.com/search?q=GRM21BR61E226ME44L</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRT21BR61E226ME13L")</f>
+        <v>http://www.octopart.com/search?q=GRT21BR61E226ME13L</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805MKX5R8BB226")</f>
+        <v>http://www.octopart.com/search?q=CC0805MKX5R8BB226</v>
+      </c>
+      <c r="N6" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM21BR61C226ME44L")</f>
+        <v>http://www.octopart.com/search?q=GRM21BR61C226ME44L</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1356,16 +1406,16 @@
       <c r="C7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="H7" s="0" t="n">
@@ -1378,6 +1428,14 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL31A106KAHNNNE")</f>
         <v>http://www.octopart.com/search?q=CL31A106KAHNNNE</v>
       </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TMK316AB7106KL-T")</f>
+        <v>http://www.octopart.com/search?q=TMK316AB7106KL-T</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TMK316BJ106ML-T")</f>
+        <v>http://www.octopart.com/search?q=TMK316BJ106ML-T</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1389,7 +1447,7 @@
       <c r="C8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="0" t="s">
@@ -1398,7 +1456,7 @@
       <c r="F8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H8" s="0" t="n">
@@ -1411,6 +1469,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM21BR61E475KA12L")</f>
         <v>http://www.octopart.com/search?q=GRM21BR61E475KA12L</v>
       </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TMK212BJ475KG-T")</f>
+        <v>http://www.octopart.com/search?q=TMK212BJ475KG-T</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1422,16 +1484,16 @@
       <c r="C9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H9" s="0" t="n">
@@ -1444,6 +1506,18 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM188R61E105KA12D")</f>
         <v>http://www.octopart.com/search?q=GRM188R61E105KA12D</v>
       </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM188R61C105KA93D")</f>
+        <v>http://www.octopart.com/search?q=GRM188R61C105KA93D</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL10B105KP8NNNC")</f>
+        <v>http://www.octopart.com/search?q=CL10B105KP8NNNC</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LMK107B7105KA-T")</f>
+        <v>http://www.octopart.com/search?q=LMK107B7105KA-T</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1464,7 +1538,7 @@
       <c r="F10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H10" s="0" t="n">
@@ -1488,16 +1562,16 @@
       <c r="C11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H11" s="0" t="n">
@@ -1510,6 +1584,18 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21B105KAFNNNE")</f>
         <v>http://www.octopart.com/search?q=CL21B105KAFNNNE</v>
       </c>
+      <c r="K11" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21B105KBFNFNE")</f>
+        <v>http://www.octopart.com/search?q=CL21B105KBFNFNE</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21A105KACLNNC")</f>
+        <v>http://www.octopart.com/search?q=CL21A105KACLNNC</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM219R71E105KA88D")</f>
+        <v>http://www.octopart.com/search?q=GRM219R71E105KA88D</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1521,7 +1607,7 @@
       <c r="C12" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="0" t="s">
@@ -1530,7 +1616,7 @@
       <c r="F12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H12" s="0" t="n">
@@ -1543,6 +1629,14 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0805C750J1GACTU")</f>
         <v>http://www.octopart.com/search?q=C0805C750J1GACTU</v>
       </c>
+      <c r="K12" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S750JV4E")</f>
+        <v>http://www.octopart.com/search?q=251R15S750JV4E</v>
+      </c>
+      <c r="L12" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=08051A750JAT2A")</f>
+        <v>http://www.octopart.com/search?q=08051A750JAT2A</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1554,7 +1648,7 @@
       <c r="C13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="0" t="s">
@@ -1563,7 +1657,7 @@
       <c r="F13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H13" s="0" t="n">
@@ -1576,6 +1670,22 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO0BN151")</f>
         <v>http://www.octopart.com/search?q=CC0805JRNPO0BN151</v>
       </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM2195C2A151JA01D")</f>
+        <v>http://www.octopart.com/search?q=GRM2195C2A151JA01D</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21C151JCANNNC")</f>
+        <v>http://www.octopart.com/search?q=CL21C151JCANNNC</v>
+      </c>
+      <c r="M13" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0805C151J1GACTU")</f>
+        <v>http://www.octopart.com/search?q=C0805C151J1GACTU</v>
+      </c>
+      <c r="N13" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S151JV4E")</f>
+        <v>http://www.octopart.com/search?q=251R15S151JV4E</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1587,7 +1697,7 @@
       <c r="C14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="E14" s="0" t="s">
@@ -1596,7 +1706,7 @@
       <c r="F14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H14" s="0" t="n">
@@ -1609,6 +1719,18 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM2165C2A161JA01D")</f>
         <v>http://www.octopart.com/search?q=GRM2165C2A161JA01D</v>
       </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21C161JCANNNC")</f>
+        <v>http://www.octopart.com/search?q=CL21C161JCANNNC</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0805C161J1GACTU")</f>
+        <v>http://www.octopart.com/search?q=C0805C161J1GACTU</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S161JV4E")</f>
+        <v>http://www.octopart.com/search?q=251R15S161JV4E</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1620,7 +1742,7 @@
       <c r="C15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E15" s="0" t="s">
@@ -1629,7 +1751,7 @@
       <c r="F15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H15" s="0" t="n">
@@ -1642,6 +1764,22 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO0BN101")</f>
         <v>http://www.octopart.com/search?q=CC0805JRNPO0BN101</v>
       </c>
+      <c r="K15" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM2195C2A101JA01D")</f>
+        <v>http://www.octopart.com/search?q=GRM2195C2A101JA01D</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21C101JCANNNC")</f>
+        <v>http://www.octopart.com/search?q=CL21C101JCANNNC</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0805C101J1GACTU")</f>
+        <v>http://www.octopart.com/search?q=C0805C101J1GACTU</v>
+      </c>
+      <c r="N15" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S101JV4E")</f>
+        <v>http://www.octopart.com/search?q=251R15S101JV4E</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1662,7 +1800,7 @@
       <c r="F16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H16" s="0" t="n">
@@ -1686,7 +1824,7 @@
       <c r="C17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="0" t="s">
@@ -1695,7 +1833,7 @@
       <c r="F17" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H17" s="0" t="n">
@@ -1708,6 +1846,22 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO0BN181")</f>
         <v>http://www.octopart.com/search?q=CC0805JRNPO0BN181</v>
       </c>
+      <c r="K17" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM2195C2A181JA01D")</f>
+        <v>http://www.octopart.com/search?q=GRM2195C2A181JA01D</v>
+      </c>
+      <c r="L17" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21C181JCANNNC")</f>
+        <v>http://www.octopart.com/search?q=CL21C181JCANNNC</v>
+      </c>
+      <c r="M17" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0805C181J1GACTU")</f>
+        <v>http://www.octopart.com/search?q=C0805C181J1GACTU</v>
+      </c>
+      <c r="N17" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S181JV4E")</f>
+        <v>http://www.octopart.com/search?q=251R15S181JV4E</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -1719,7 +1873,7 @@
       <c r="C18" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="0" t="s">
@@ -1728,7 +1882,7 @@
       <c r="F18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H18" s="0" t="n">
@@ -1741,6 +1895,14 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO0BN271")</f>
         <v>http://www.octopart.com/search?q=CC0805JRNPO0BN271</v>
       </c>
+      <c r="K18" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM2195C2A271JA01D")</f>
+        <v>http://www.octopart.com/search?q=GRM2195C2A271JA01D</v>
+      </c>
+      <c r="L18" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S271JV4E")</f>
+        <v>http://www.octopart.com/search?q=251R15S271JV4E</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -1761,7 +1923,7 @@
       <c r="F19" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H19" s="0" t="n">
@@ -1794,7 +1956,7 @@
       <c r="F20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H20" s="0" t="n">
@@ -1827,7 +1989,7 @@
       <c r="F21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H21" s="0" t="n">
@@ -1837,6 +1999,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=DIKAVS DC005")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=DIKAVS DC005</v>
+      </c>
+      <c r="K21" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PJ-102AH")</f>
         <v>http://www.octopart.com/search?q=PJ-102AH</v>
       </c>
@@ -1860,7 +2026,7 @@
       <c r="F22" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H22" s="0" t="n">
@@ -1893,7 +2059,7 @@
       <c r="F23" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H23" s="0" t="n">
@@ -1903,6 +2069,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PJ-307")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=PJ-307</v>
+      </c>
+      <c r="K23" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SJ1-3525N")</f>
         <v>http://www.octopart.com/search?q=SJ1-3525N</v>
       </c>
@@ -1926,7 +2096,7 @@
       <c r="F24" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="5" t="s">
         <v>83</v>
       </c>
       <c r="H24" s="0" t="n">
@@ -1959,7 +2129,7 @@
       <c r="F25" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="5" t="s">
         <v>87</v>
       </c>
       <c r="H25" s="0" t="n">
@@ -1983,7 +2153,7 @@
       <c r="C26" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E26" s="0" t="s">
@@ -1992,7 +2162,7 @@
       <c r="F26" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="5" t="s">
         <v>90</v>
       </c>
       <c r="H26" s="0" t="n">
@@ -2005,6 +2175,14 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=SM05.TCT")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=SM05.TCT</v>
       </c>
+      <c r="K26" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SM05.TCT")</f>
+        <v>http://www.octopart.com/search?q=SM05.TCT</v>
+      </c>
+      <c r="L26" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=tpd2e009")</f>
+        <v>http://www.octopart.com/search?q=tpd2e009</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -2025,7 +2203,7 @@
       <c r="F27" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="5" t="s">
         <v>93</v>
       </c>
       <c r="H27" s="0" t="n">
@@ -2038,6 +2216,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=SMBJ18CA")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=SMBJ18CA</v>
       </c>
+      <c r="K27" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SMBJ18CA")</f>
+        <v>http://www.octopart.com/search?q=SMBJ18CA</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -2058,7 +2240,7 @@
       <c r="F28" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H28" s="0" t="n">
@@ -2091,7 +2273,7 @@
       <c r="F29" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>100</v>
       </c>
       <c r="H29" s="0" t="n">
@@ -2104,6 +2286,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MF-LSMF300/24X-2")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=MF-LSMF300/24X-2</v>
       </c>
+      <c r="K29" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MF-LSMF300/24X-2")</f>
+        <v>http://www.octopart.com/search?q=MF-LSMF300/24X-2</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -2121,10 +2307,10 @@
       <c r="E30" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G30" s="4" t="n">
+      <c r="G30" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H30" s="0" t="n">
@@ -2148,16 +2334,16 @@
       <c r="C31" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>105</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H31" s="0" t="n">
@@ -2170,6 +2356,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603JR-070RL")</f>
         <v>http://www.octopart.com/search?q=RC0603JR-070RL</v>
       </c>
+      <c r="K31" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-J/-000ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-J/-000ELF</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -2181,7 +2371,7 @@
       <c r="C32" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>108</v>
       </c>
       <c r="E32" s="0" t="s">
@@ -2190,7 +2380,7 @@
       <c r="F32" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H32" s="0" t="n">
@@ -2200,8 +2390,16 @@
         <v>1</v>
       </c>
       <c r="J32" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EC2-3NU")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=EC2-3NU</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EC2-3NJ")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=EC2-3NJ</v>
+      </c>
+      <c r="K32" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EC2-3NU")</f>
+        <v>http://www.octopart.com/search?q=EC2-3NU</v>
+      </c>
+      <c r="L32" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EC2-3NJ")</f>
+        <v>http://www.octopart.com/search?q=EC2-3NJ</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2223,7 +2421,7 @@
       <c r="F33" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="5" t="s">
         <v>113</v>
       </c>
       <c r="H33" s="0" t="n">
@@ -2256,7 +2454,7 @@
       <c r="F34" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="5" t="s">
         <v>113</v>
       </c>
       <c r="H34" s="0" t="n">
@@ -2289,7 +2487,7 @@
       <c r="F35" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="G35" s="4" t="n">
+      <c r="G35" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H35" s="0" t="n">
@@ -2322,7 +2520,7 @@
       <c r="F36" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="G36" s="4" t="n">
+      <c r="G36" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H36" s="0" t="n">
@@ -2355,7 +2553,7 @@
       <c r="F37" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H37" s="0" t="n">
@@ -2388,7 +2586,7 @@
       <c r="F38" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="5" t="s">
         <v>90</v>
       </c>
       <c r="H38" s="0" t="n">
@@ -2421,7 +2619,7 @@
       <c r="F39" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="5" t="s">
         <v>90</v>
       </c>
       <c r="H39" s="0" t="n">
@@ -2434,6 +2632,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=NUD3124LT1G")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=NUD3124LT1G</v>
       </c>
+      <c r="K39" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=NUD3124LT1G")</f>
+        <v>http://www.octopart.com/search?q=NUD3124LT1G</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -2454,7 +2656,7 @@
       <c r="F40" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="5" t="s">
         <v>135</v>
       </c>
       <c r="H40" s="0" t="n">
@@ -2487,7 +2689,7 @@
       <c r="F41" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="5" t="s">
         <v>90</v>
       </c>
       <c r="H41" s="0" t="n">
@@ -2500,6 +2702,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MCP9700T-E/TT")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=MCP9700T-E/TT</v>
       </c>
+      <c r="K41" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MCP9700T-E/TT")</f>
+        <v>http://www.octopart.com/search?q=MCP9700T-E/TT</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -2511,16 +2717,16 @@
       <c r="C42" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="4" t="s">
         <v>140</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G42" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H42" s="0" t="n">
@@ -2533,6 +2739,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0733RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0733RL</v>
       </c>
+      <c r="K42" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-33R0ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-33R0ELF</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -2544,16 +2754,16 @@
       <c r="C43" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="4" t="s">
         <v>143</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="4" t="n">
+      <c r="G43" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H43" s="0" t="n">
@@ -2566,6 +2776,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0710KL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0710KL</v>
       </c>
+      <c r="K43" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1002HLF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-1002HLF</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -2586,7 +2800,7 @@
       <c r="F44" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="4" t="n">
+      <c r="G44" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H44" s="0" t="n">
@@ -2619,7 +2833,7 @@
       <c r="F45" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="G45" s="4" t="n">
+      <c r="G45" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H45" s="0" t="n">
@@ -2652,7 +2866,7 @@
       <c r="F46" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="G46" s="4" t="n">
+      <c r="G46" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H46" s="0" t="n">
@@ -2676,7 +2890,7 @@
       <c r="C47" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="4" t="s">
         <v>155</v>
       </c>
       <c r="E47" s="0" t="s">
@@ -2685,7 +2899,7 @@
       <c r="F47" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="G47" s="4" t="n">
+      <c r="G47" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H47" s="0" t="n">
@@ -2698,6 +2912,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0720KL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0720KL</v>
       </c>
+      <c r="K47" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-2002ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-2002ELF</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -2718,7 +2936,7 @@
       <c r="F48" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G48" s="4" t="n">
+      <c r="G48" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H48" s="0" t="n">
@@ -2748,10 +2966,10 @@
       <c r="E49" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G49" s="4" t="n">
+      <c r="G49" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H49" s="0" t="n">
@@ -2784,7 +3002,7 @@
       <c r="F50" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="G50" s="4" t="n">
+      <c r="G50" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H50" s="0" t="n">
@@ -2817,7 +3035,7 @@
       <c r="F51" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="G51" s="4" t="n">
+      <c r="G51" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H51" s="0" t="n">
@@ -2841,7 +3059,7 @@
       <c r="C52" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="4" t="s">
         <v>170</v>
       </c>
       <c r="E52" s="0" t="s">
@@ -2850,7 +3068,7 @@
       <c r="F52" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="G52" s="4" t="n">
+      <c r="G52" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H52" s="0" t="n">
@@ -2863,6 +3081,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0775RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0775RL</v>
       </c>
+      <c r="K52" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-75R0ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-75R0ELF</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -2874,16 +3096,16 @@
       <c r="C53" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="4" t="s">
         <v>173</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G53" s="4" t="n">
+      <c r="G53" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H53" s="0" t="n">
@@ -2896,6 +3118,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-074K7L")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-074K7L</v>
       </c>
+      <c r="K53" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-4701ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-4701ELF</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -2907,7 +3133,7 @@
       <c r="C54" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E54" s="0" t="s">
@@ -2916,7 +3142,7 @@
       <c r="F54" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="G54" s="4" t="n">
+      <c r="G54" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H54" s="0" t="n">
@@ -2929,6 +3155,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-071K8L")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-071K8L</v>
       </c>
+      <c r="K54" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1801ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-1801ELF</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -2949,7 +3179,7 @@
       <c r="F55" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="G55" s="4" t="n">
+      <c r="G55" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H55" s="0" t="n">
@@ -2973,7 +3203,7 @@
       <c r="C56" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="4" t="s">
         <v>182</v>
       </c>
       <c r="E56" s="0" t="s">
@@ -2982,7 +3212,7 @@
       <c r="F56" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="G56" s="4" t="n">
+      <c r="G56" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H56" s="0" t="n">
@@ -2995,6 +3225,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0722RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0722RL</v>
       </c>
+      <c r="K56" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-22R0ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-22R0ELF</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -3006,16 +3240,16 @@
       <c r="C57" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="4" t="s">
         <v>185</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G57" s="5" t="n">
         <v>805</v>
       </c>
       <c r="H57" s="0" t="n">
@@ -3028,6 +3262,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0805FR-0712RL")</f>
         <v>http://www.octopart.com/search?q=RC0805FR-0712RL</v>
       </c>
+      <c r="K57" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ERJ-6ENF12R0V")</f>
+        <v>http://www.octopart.com/search?q=ERJ-6ENF12R0V</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -3048,7 +3286,7 @@
       <c r="F58" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="G58" s="4" t="n">
+      <c r="G58" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H58" s="0" t="n">
@@ -3072,7 +3310,7 @@
       <c r="C59" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="4" t="s">
         <v>191</v>
       </c>
       <c r="E59" s="0" t="s">
@@ -3081,7 +3319,7 @@
       <c r="F59" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="G59" s="4" t="n">
+      <c r="G59" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H59" s="0" t="n">
@@ -3094,6 +3332,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07330RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-07330RL</v>
       </c>
+      <c r="K59" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-3300ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-3300ELF</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -3105,16 +3347,16 @@
       <c r="C60" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="4" t="s">
         <v>194</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G60" s="4" t="n">
+      <c r="G60" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H60" s="0" t="n">
@@ -3127,6 +3369,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-071KL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-071KL</v>
       </c>
+      <c r="K60" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1001HLF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-1001HLF</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -3147,7 +3393,7 @@
       <c r="F61" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="G61" s="4" t="n">
+      <c r="G61" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H61" s="0" t="n">
@@ -3180,7 +3426,7 @@
       <c r="F62" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="G62" s="4" t="n">
+      <c r="G62" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H62" s="0" t="n">
@@ -3204,7 +3450,7 @@
       <c r="C63" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="4" t="s">
         <v>203</v>
       </c>
       <c r="E63" s="0" t="s">
@@ -3213,7 +3459,7 @@
       <c r="F63" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="G63" s="4" t="n">
+      <c r="G63" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H63" s="0" t="n">
@@ -3226,6 +3472,14 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07100RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-07100RL</v>
       </c>
+      <c r="K63" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1000ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-1000ELF</v>
+      </c>
+      <c r="L63" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AC0603FR-07100RL")</f>
+        <v>http://www.octopart.com/search?q=AC0603FR-07100RL</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -3237,16 +3491,16 @@
       <c r="C64" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="4" t="s">
         <v>206</v>
       </c>
       <c r="E64" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="G64" s="4" t="n">
+      <c r="G64" s="5" t="n">
         <v>603</v>
       </c>
       <c r="H64" s="0" t="n">
@@ -3259,6 +3513,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07270RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-07270RL</v>
       </c>
+      <c r="K64" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-2700ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-2700ELF</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -3270,7 +3528,7 @@
       <c r="C65" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="4" t="s">
         <v>209</v>
       </c>
       <c r="E65" s="0" t="s">
@@ -3279,7 +3537,7 @@
       <c r="F65" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="G65" s="4" t="n">
+      <c r="G65" s="5" t="n">
         <v>1206</v>
       </c>
       <c r="H65" s="0" t="n">
@@ -3292,6 +3550,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RL1206FR-070R04L")</f>
         <v>http://www.octopart.com/search?q=RL1206FR-070R04L</v>
       </c>
+      <c r="K65" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PE1206FRM070R04L")</f>
+        <v>http://www.octopart.com/search?q=PE1206FRM070R04L</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -3303,7 +3565,7 @@
       <c r="C66" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="4" t="s">
         <v>212</v>
       </c>
       <c r="E66" s="0" t="s">
@@ -3312,7 +3574,7 @@
       <c r="F66" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="G66" s="5" t="s">
         <v>214</v>
       </c>
       <c r="H66" s="0" t="n">
@@ -3325,6 +3587,18 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MABAES0060")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=MABAES0060</v>
       </c>
+      <c r="K66" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MABAES0060")</f>
+        <v>http://www.octopart.com/search?q=MABAES0060</v>
+      </c>
+      <c r="L66" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PWB1010-1LB")</f>
+        <v>http://www.octopart.com/search?q=PWB1010-1LB</v>
+      </c>
+      <c r="M66" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TC1-1TG2+")</f>
+        <v>http://www.octopart.com/search?q=TC1-1TG2+</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
@@ -3336,7 +3610,7 @@
       <c r="C67" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="4" t="s">
         <v>216</v>
       </c>
       <c r="E67" s="0" t="s">
@@ -3345,7 +3619,7 @@
       <c r="F67" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G67" s="5" t="s">
         <v>214</v>
       </c>
       <c r="H67" s="0" t="n">
@@ -3358,6 +3632,10 @@
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MABA-010143-FLUX18")</f>
         <v>http://www.octopart.com/search?q=MABA-010143-FLUX18</v>
       </c>
+      <c r="K67" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=WBC8-1LB")</f>
+        <v>http://www.octopart.com/search?q=WBC8-1LB</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
@@ -3378,11 +3656,11 @@
       <c r="F68" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="G68" s="4" t="s">
+      <c r="G68" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H68" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I68" s="0" t="n">
         <v>1</v>
@@ -3402,7 +3680,7 @@
       <c r="C69" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="4" t="s">
         <v>222</v>
       </c>
       <c r="E69" s="0" t="s">
@@ -3411,7 +3689,7 @@
       <c r="F69" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="G69" s="5" t="s">
         <v>224</v>
       </c>
       <c r="H69" s="0" t="n">
@@ -3424,6 +3702,18 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=S25FL116K0XMFI041")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=S25FL116K0XMFI041</v>
       </c>
+      <c r="K69" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=W25Q16JVSNIQ")</f>
+        <v>http://www.octopart.com/search?q=W25Q16JVSNIQ</v>
+      </c>
+      <c r="L69" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=S25FL116K0XMFI043")</f>
+        <v>http://www.octopart.com/search?q=S25FL116K0XMFI043</v>
+      </c>
+      <c r="M69" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=S25FL116K0XMFI041")</f>
+        <v>http://www.octopart.com/search?q=S25FL116K0XMFI041</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
@@ -3444,7 +3734,7 @@
       <c r="F70" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="G70" s="4" t="s">
+      <c r="G70" s="5" t="s">
         <v>228</v>
       </c>
       <c r="H70" s="0" t="n">
@@ -3457,6 +3747,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EP4CE22E22C8N")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=EP4CE22E22C8N</v>
       </c>
+      <c r="K70" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EP4CE22E22C8N")</f>
+        <v>http://www.octopart.com/search?q=EP4CE22E22C8N</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
@@ -3477,7 +3771,7 @@
       <c r="F71" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="G71" s="4" t="s">
+      <c r="G71" s="5" t="s">
         <v>232</v>
       </c>
       <c r="H71" s="0" t="n">
@@ -3490,6 +3784,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=st1s10")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=st1s10</v>
       </c>
+      <c r="K71" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ST1S10PHR")</f>
+        <v>http://www.octopart.com/search?q=ST1S10PHR</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
@@ -3501,7 +3799,7 @@
       <c r="C72" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="4" t="s">
         <v>234</v>
       </c>
       <c r="E72" s="0" t="s">
@@ -3510,7 +3808,7 @@
       <c r="F72" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="G72" s="4" t="s">
+      <c r="G72" s="5" t="s">
         <v>236</v>
       </c>
       <c r="H72" s="0" t="n">
@@ -3523,6 +3821,14 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=KSZ9031")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=KSZ9031</v>
       </c>
+      <c r="K72" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=KSZ9031RNXCC")</f>
+        <v>http://www.octopart.com/search?q=KSZ9031RNXCC</v>
+      </c>
+      <c r="L72" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=KSZ9031RNXCA")</f>
+        <v>http://www.octopart.com/search?q=KSZ9031RNXCA</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
@@ -3543,7 +3849,7 @@
       <c r="F73" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="G73" s="4" t="s">
+      <c r="G73" s="5" t="s">
         <v>240</v>
       </c>
       <c r="H73" s="0" t="n">
@@ -3576,7 +3882,7 @@
       <c r="F74" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="G74" s="4" t="s">
+      <c r="G74" s="5" t="s">
         <v>244</v>
       </c>
       <c r="H74" s="0" t="n">
@@ -3589,6 +3895,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=AD9866BCPZ")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=AD9866BCPZ</v>
       </c>
+      <c r="K74" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AD9866BCPZ")</f>
+        <v>http://www.octopart.com/search?q=AD9866BCPZ</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
@@ -3609,7 +3919,7 @@
       <c r="F75" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="G75" s="4" t="s">
+      <c r="G75" s="5" t="s">
         <v>232</v>
       </c>
       <c r="H75" s="0" t="n">
@@ -3622,6 +3932,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=OPA2677")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=OPA2677</v>
       </c>
+      <c r="K75" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=OPA2677IDDA")</f>
+        <v>http://www.octopart.com/search?q=OPA2677IDDA</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
@@ -3633,7 +3947,7 @@
       <c r="C76" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="4" t="s">
         <v>249</v>
       </c>
       <c r="E76" s="0" t="s">
@@ -3642,7 +3956,7 @@
       <c r="F76" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="G76" s="4" t="s">
+      <c r="G76" s="5" t="s">
         <v>251</v>
       </c>
       <c r="H76" s="0" t="n">
@@ -3655,6 +3969,18 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=pe4259")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=pe4259</v>
       </c>
+      <c r="K76" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=4259-63")</f>
+        <v>http://www.octopart.com/search?q=4259-63</v>
+      </c>
+      <c r="L76" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=4239-52")</f>
+        <v>http://www.octopart.com/search?q=4239-52</v>
+      </c>
+      <c r="M76" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PE42421SCAA")</f>
+        <v>http://www.octopart.com/search?q=PE42421SCAA</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
@@ -3675,7 +4001,7 @@
       <c r="F77" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="G77" s="4" t="s">
+      <c r="G77" s="5" t="s">
         <v>232</v>
       </c>
       <c r="H77" s="0" t="n">
@@ -3708,7 +4034,7 @@
       <c r="F78" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="G78" s="4" t="s">
+      <c r="G78" s="5" t="s">
         <v>258</v>
       </c>
       <c r="H78" s="0" t="n">
@@ -3741,7 +4067,7 @@
       <c r="F79" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="G79" s="4" t="s">
+      <c r="G79" s="5" t="s">
         <v>262</v>
       </c>
       <c r="H79" s="0" t="n">
@@ -3774,7 +4100,7 @@
       <c r="F80" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="G80" s="4" t="s">
+      <c r="G80" s="5" t="s">
         <v>266</v>
       </c>
       <c r="H80" s="0" t="n">
@@ -3807,7 +4133,7 @@
       <c r="F81" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="5" t="s">
         <v>269</v>
       </c>
       <c r="H81" s="0" t="n">
@@ -3820,6 +4146,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=TPS73025DBVR")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=TPS73025DBVR</v>
       </c>
+      <c r="K81" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TPS73025DBVR")</f>
+        <v>http://www.octopart.com/search?q=TPS73025DBVR</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
@@ -3840,7 +4170,7 @@
       <c r="F82" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="5" t="s">
         <v>269</v>
       </c>
       <c r="H82" s="0" t="n">
@@ -3873,11 +4203,11 @@
       <c r="F83" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="G83" s="4" t="s">
+      <c r="G83" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H83" s="0" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I83" s="0" t="n">
         <v>1</v>
@@ -3886,6 +4216,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG</v>
       </c>
+      <c r="K83" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=400R0111-24-9")</f>
+        <v>http://www.octopart.com/search?q=400R0111-24-9</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
@@ -3906,7 +4240,7 @@
       <c r="F84" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="G84" s="4" t="s">
+      <c r="G84" s="5" t="s">
         <v>279</v>
       </c>
       <c r="H84" s="0" t="n">
@@ -3919,6 +4253,10 @@
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=25mhz 3.2x2.5 passive")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=25mhz 3.2x2.5 passive</v>
       </c>
+      <c r="K84" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=NX3225SA-25.000M-STD-CSR-3")</f>
+        <v>http://www.octopart.com/search?q=NX3225SA-25.000M-STD-CSR-3</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
@@ -3939,7 +4277,7 @@
       <c r="F85" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="G85" s="4" t="s">
+      <c r="G85" s="5" t="s">
         <v>283</v>
       </c>
       <c r="H85" s="0" t="n">
@@ -3953,65 +4291,77 @@
         <v>http://www.octopart.com/search?q=ASTXR-12-38.400MHZ-514054-T</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G86" s="5"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="6" t="s">
         <v>284</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="6" t="s">
         <v>285</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G87" s="5"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6" t="s">
         <v>286</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>368</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="6" t="s">
         <v>287</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="6" t="s">
         <v>288</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>1093</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="6" t="s">
         <v>289</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G89" s="5"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>290</v>
       </c>
       <c r="B91" s="1"/>
+      <c r="G91" s="5"/>
     </row>
     <row r="92" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="J1:N1"/>
     <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="A92:D92"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Build9 final changes before submission
</commit_message>
<xml_diff>
--- a/hardware/hl/bom/bom.assembly.xlsx
+++ b/hardware/hl/bom/bom.assembly.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="301">
   <si>
     <t xml:space="preserve">Line</t>
   </si>
@@ -267,12 +267,13 @@
     <t xml:space="preserve">C56</t>
   </si>
   <si>
-    <t xml:space="preserve">270pF 0805NP0&gt;=50V&lt;=5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0805JRNPO0BN271
-GRM2195C2A271JA01D
-251R15S271JV4E</t>
+    <t xml:space="preserve">390pF 0805NP0&gt;=50V&lt;=5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0805JRNPO0BN391
+CL21C391JBANNNC
+CC0805JRNPO9BN391
+C0805C391J5GACTU</t>
   </si>
   <si>
     <t xml:space="preserve">C84</t>
@@ -287,6 +288,18 @@
     <t xml:space="preserve">C87</t>
   </si>
   <si>
+    <t xml:space="preserve">SMA Straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-1814832-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL1,CL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom</t>
+  </si>
+  <si>
     <t xml:space="preserve">2x5 M 0.1in</t>
   </si>
   <si>
@@ -294,9 +307,6 @@
   </si>
   <si>
     <t xml:space="preserve">CN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom</t>
   </si>
   <si>
     <t xml:space="preserve">Power</t>
@@ -405,6 +415,24 @@
 FB28,FB30</t>
   </si>
   <si>
+    <t xml:space="preserve">14X14mm Raspberry Pi Heatsink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rp14x14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9X9mm Raspberry Pi Heatsink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rp9x9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS7</t>
+  </si>
+  <si>
     <t xml:space="preserve">0Ohm 0603&lt;=5%&gt;=1/10W</t>
   </si>
   <si>
@@ -535,9 +563,9 @@
   </si>
   <si>
     <t xml:space="preserve">R2,R3,R4,R5,R6,R7,
-R14,R21,R22,R23,R24,
-R25,R27,R28,R29,R131,
-R132</t>
+R13,R14,R16,R21,R22,
+R23,R24,R25,R27,R28,
+R29,R131,R132</t>
   </si>
   <si>
     <t xml:space="preserve">2.2 0603&lt;=5%&gt;=1/10W</t>
@@ -1006,11 +1034,11 @@
   </si>
   <si>
     <t xml:space="preserve">B55,B104,B107,C42,C47,C54,C55,C58,C59,C79,C80,C82,C83,C85,C148,
-C149,CL1,CL2,CL3,CL4,CL5,CL6,CL7,CL8,CL10,CN7,CN8,CN9,CN10,D6,
-D7,DB1,DB2,DB3,DB6,DB8,DB9,DB11,DB12,DB13,DB14,DB15,DB17,DB20,
-DB23,DB27,J3,J4,J6,J7,J8,J12,J14,J16,J20,R8,R9,R13,R16,R17,R36,
-R38,R60,R93,R96,R97,R98,R104,R112,R115,R128,R129,R135,RF1,RF2,
-RF3,RF4,RF5,RF6,RF7,X3</t>
+C149,CL3,CL4,CL5,CL6,CL7,CL8,CL10,CN7,CN8,CN9,CN10,D6,D7,DB1,
+DB2,DB3,DB6,DB8,DB9,DB11,DB12,DB13,DB14,DB15,DB17,DB20,DB23,DB27,
+J3,J4,J6,J7,J8,J12,J14,J16,J20,R8,R9,R17,R36,R38,R60,R93,R96,
+R97,R98,R104,R112,R115,R128,R129,R135,RF1,RF2,RF3,RF4,RF5,RF6,
+RF7,X3</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1124,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1109,16 +1137,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1142,32 +1162,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N92"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.969387755102"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0102040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.24489795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="58.4948979591837"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="53.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9234693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.18877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.3673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="72.9387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="56.4540816326531"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="49.9183673469388"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="50.1989795918367"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="50.4795918367347"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +1206,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1203,7 +1223,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="248.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="247.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -1213,16 +1233,16 @@
       <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -1240,7 +1260,7 @@
         <v>http://www.octopart.com/search?q=C1608X7R1E104K080AA</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -1250,16 +1270,16 @@
       <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -1296,7 +1316,7 @@
       <c r="F4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="0" t="n">
         <v>1206</v>
       </c>
       <c r="H4" s="0" t="n">
@@ -1310,7 +1330,7 @@
         <v>http://www.octopart.com/search?q=GRM31CR60J107ME39K</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -1320,7 +1340,7 @@
       <c r="C5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -1329,7 +1349,7 @@
       <c r="F5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -1347,7 +1367,7 @@
         <v>http://www.octopart.com/search?q=C0603C472K5RACTU</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -1357,16 +1377,16 @@
       <c r="C6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H6" s="0" t="n">
@@ -1396,7 +1416,7 @@
         <v>http://www.octopart.com/search?q=GRM21BR61C226ME44L</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -1406,16 +1426,16 @@
       <c r="C7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="0" t="n">
         <v>1206</v>
       </c>
       <c r="H7" s="0" t="n">
@@ -1437,7 +1457,7 @@
         <v>http://www.octopart.com/search?q=TMK316BJ106ML-T</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -1447,7 +1467,7 @@
       <c r="C8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="0" t="s">
@@ -1456,7 +1476,7 @@
       <c r="F8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H8" s="0" t="n">
@@ -1474,7 +1494,7 @@
         <v>http://www.octopart.com/search?q=TMK212BJ475KG-T</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -1484,16 +1504,16 @@
       <c r="C9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H9" s="0" t="n">
@@ -1538,7 +1558,7 @@
       <c r="F10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H10" s="0" t="n">
@@ -1552,7 +1572,7 @@
         <v>http://www.octopart.com/search?q=CC0603JRNPO9BN150</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -1562,16 +1582,16 @@
       <c r="C11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H11" s="0" t="n">
@@ -1597,7 +1617,7 @@
         <v>http://www.octopart.com/search?q=GRM219R71E105KA88D</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
@@ -1607,7 +1627,7 @@
       <c r="C12" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="0" t="s">
@@ -1616,7 +1636,7 @@
       <c r="F12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H12" s="0" t="n">
@@ -1638,7 +1658,7 @@
         <v>http://www.octopart.com/search?q=08051A750JAT2A</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
@@ -1648,7 +1668,7 @@
       <c r="C13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="0" t="s">
@@ -1657,7 +1677,7 @@
       <c r="F13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H13" s="0" t="n">
@@ -1687,7 +1707,7 @@
         <v>http://www.octopart.com/search?q=251R15S151JV4E</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -1697,7 +1717,7 @@
       <c r="C14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E14" s="0" t="s">
@@ -1706,7 +1726,7 @@
       <c r="F14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H14" s="0" t="n">
@@ -1732,7 +1752,7 @@
         <v>http://www.octopart.com/search?q=251R15S161JV4E</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
@@ -1742,7 +1762,7 @@
       <c r="C15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E15" s="0" t="s">
@@ -1751,7 +1771,7 @@
       <c r="F15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H15" s="0" t="n">
@@ -1800,7 +1820,7 @@
       <c r="F16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H16" s="0" t="n">
@@ -1814,7 +1834,7 @@
         <v>http://www.octopart.com/search?q=CC0805JRNPO9BN100</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -1824,7 +1844,7 @@
       <c r="C17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="0" t="s">
@@ -1833,7 +1853,7 @@
       <c r="F17" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H17" s="0" t="n">
@@ -1863,7 +1883,7 @@
         <v>http://www.octopart.com/search?q=251R15S181JV4E</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -1873,7 +1893,7 @@
       <c r="C18" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E18" s="0" t="s">
@@ -1882,7 +1902,7 @@
       <c r="F18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H18" s="0" t="n">
@@ -1892,16 +1912,20 @@
         <v>1</v>
       </c>
       <c r="J18" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO0BN271")</f>
-        <v>http://www.octopart.com/search?q=CC0805JRNPO0BN271</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO0BN391")</f>
+        <v>http://www.octopart.com/search?q=CC0805JRNPO0BN391</v>
       </c>
       <c r="K18" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=GRM2195C2A271JA01D")</f>
-        <v>http://www.octopart.com/search?q=GRM2195C2A271JA01D</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CL21C391JBANNNC")</f>
+        <v>http://www.octopart.com/search?q=CL21C391JBANNNC</v>
       </c>
       <c r="L18" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=251R15S271JV4E")</f>
-        <v>http://www.octopart.com/search?q=251R15S271JV4E</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CC0805JRNPO9BN391")</f>
+        <v>http://www.octopart.com/search?q=CC0805JRNPO9BN391</v>
+      </c>
+      <c r="M18" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=C0805C391J5GACTU")</f>
+        <v>http://www.octopart.com/search?q=C0805C391J5GACTU</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,7 +1947,7 @@
       <c r="F19" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="0" t="n">
         <v>805</v>
       </c>
       <c r="H19" s="0" t="n">
@@ -1956,18 +1980,18 @@
       <c r="F20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="0" t="s">
         <v>70</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=67997-410HLF")</f>
-        <v>http://www.octopart.com/search?q=67997-410HLF</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=5-1814832-1")</f>
+        <v>http://www.octopart.com/search?q=5-1814832-1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,22 +2013,18 @@
       <c r="F21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="0" t="s">
         <v>70</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J21" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=DIKAVS DC005")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=DIKAVS DC005</v>
-      </c>
-      <c r="K21" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PJ-102AH")</f>
-        <v>http://www.octopart.com/search?q=PJ-102AH</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=67997-410HLF")</f>
+        <v>http://www.octopart.com/search?q=67997-410HLF</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,23 +2041,27 @@
         <v>75</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="0" t="s">
         <v>70</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J22" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=L829-1J1T-43")</f>
-        <v>http://www.octopart.com/search?q=L829-1J1T-43</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=DIKAVS DC005")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=DIKAVS DC005</v>
+      </c>
+      <c r="K22" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PJ-102AH")</f>
+        <v>http://www.octopart.com/search?q=PJ-102AH</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,27 +2078,23 @@
         <v>78</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="0" t="s">
         <v>70</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J23" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PJ-307")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=PJ-307</v>
-      </c>
-      <c r="K23" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SJ1-3525N")</f>
-        <v>http://www.octopart.com/search?q=SJ1-3525N</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=L829-1J1T-43")</f>
+        <v>http://www.octopart.com/search?q=L829-1J1T-43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,23 +2111,27 @@
         <v>81</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>83</v>
+      <c r="G24" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J24" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CDSOD323-T05LC")</f>
-        <v>http://www.octopart.com/search?q=CDSOD323-T05LC</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PJ-307")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=PJ-307</v>
+      </c>
+      <c r="K24" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SJ1-3525N")</f>
+        <v>http://www.octopart.com/search?q=SJ1-3525N</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2118,107 +2142,103 @@
         <v>17</v>
       </c>
       <c r="C25" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="H25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CDSOD323-T05LC")</f>
+        <v>http://www.octopart.com/search?q=CDSOD323-T05LC</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I25" s="0" t="n">
+      <c r="D26" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="J25" s="0" t="str">
+      <c r="J26" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LTST-S220KFKT")</f>
         <v>http://www.octopart.com/search?q=LTST-S220KFKT</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="0" t="s">
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="0" t="n">
+      <c r="F27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J26" s="0" t="str">
+      <c r="I27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=SM05.TCT")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=SM05.TCT</v>
       </c>
-      <c r="K26" s="0" t="str">
+      <c r="K27" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SM05.TCT")</f>
         <v>http://www.octopart.com/search?q=SM05.TCT</v>
       </c>
-      <c r="L26" s="0" t="str">
+      <c r="L27" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=tpd2e009")</f>
         <v>http://www.octopart.com/search?q=tpd2e009</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J27" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=SMBJ18CA")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=SMBJ18CA</v>
-      </c>
-      <c r="K27" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SMBJ18CA")</f>
-        <v>http://www.octopart.com/search?q=SMBJ18CA</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,29 +2249,33 @@
         <v>17</v>
       </c>
       <c r="C28" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="E28" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="G28" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="H28" s="0" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J28" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PRPC040SAAN-RC")</f>
-        <v>http://www.octopart.com/search?q=PRPC040SAAN-RC</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=SMBJ18CA")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=SMBJ18CA</v>
+      </c>
+      <c r="K28" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SMBJ18CA")</f>
+        <v>http://www.octopart.com/search?q=SMBJ18CA</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,100 +2292,96 @@
         <v>98</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PRPC040SAAN-RC")</f>
+        <v>http://www.octopart.com/search?q=PRPC040SAAN-RC</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J29" s="0" t="str">
+      <c r="D30" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MF-LSMF300/24X-2")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=MF-LSMF300/24X-2</v>
       </c>
-      <c r="K29" s="0" t="str">
+      <c r="K30" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MF-LSMF300/24X-2")</f>
         <v>http://www.octopart.com/search?q=MF-LSMF300/24X-2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="5" t="n">
+    <row r="31" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I30" s="0" t="n">
+      <c r="H31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="J30" s="0" t="str">
+      <c r="J31" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MPZ1608S601ATA00")</f>
         <v>http://www.octopart.com/search?q=MPZ1608S601ATA00</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>21903</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" s="5" t="n">
-        <v>603</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="J31" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603JR-070RL")</f>
-        <v>http://www.octopart.com/search?q=RC0603JR-070RL</v>
-      </c>
-      <c r="K31" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-J/-000ELF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-J/-000ELF</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
@@ -2371,35 +2391,31 @@
       <c r="C32" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="0" t="s">
         <v>108</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="G32" s="0" t="s">
         <v>70</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J32" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EC2-3NJ")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=EC2-3NJ</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=raspberry pi heat sink")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=raspberry pi heat sink</v>
       </c>
       <c r="K32" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EC2-3NU")</f>
-        <v>http://www.octopart.com/search?q=EC2-3NU</v>
-      </c>
-      <c r="L32" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EC2-3NJ")</f>
-        <v>http://www.octopart.com/search?q=EC2-3NJ</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=rp14x14")</f>
+        <v>http://www.octopart.com/search?q=rp14x14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,59 +2432,67 @@
         <v>111</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>113</v>
+      <c r="G33" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I33" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SRR4528A-3R3Y")</f>
-        <v>http://www.octopart.com/search?q=SRR4528A-3R3Y</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=raspberry pi heat sink")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=raspberry pi heat sink</v>
+      </c>
+      <c r="K33" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=rp9x9")</f>
+        <v>http://www.octopart.com/search?q=rp9x9</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>17</v>
+      <c r="B34" s="0" t="n">
+        <v>21903</v>
       </c>
       <c r="C34" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="E34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E34" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>113</v>
+      <c r="G34" s="0" t="n">
+        <v>603</v>
       </c>
       <c r="H34" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J34" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SRR4528A-2R2Y")</f>
-        <v>http://www.octopart.com/search?q=SRR4528A-2R2Y</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603JR-070RL")</f>
+        <v>http://www.octopart.com/search?q=RC0603JR-070RL</v>
+      </c>
+      <c r="K34" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-J/-000ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-J/-000ELF</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
@@ -2476,29 +2500,37 @@
         <v>17</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>118</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="G35" s="5" t="n">
-        <v>805</v>
+        <v>118</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J35" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LQW2BASR24J00L")</f>
-        <v>http://www.octopart.com/search?q=LQW2BASR24J00L</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EC2-3NJ")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=EC2-3NJ</v>
+      </c>
+      <c r="K35" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EC2-3NU")</f>
+        <v>http://www.octopart.com/search?q=EC2-3NU</v>
+      </c>
+      <c r="L35" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EC2-3NJ")</f>
+        <v>http://www.octopart.com/search?q=EC2-3NJ</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,29 +2541,29 @@
         <v>17</v>
       </c>
       <c r="C36" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>121</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F36" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="G36" s="5" t="n">
-        <v>805</v>
-      </c>
       <c r="H36" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J36" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LQW2BASR27J00L")</f>
-        <v>http://www.octopart.com/search?q=LQW2BASR27J00L</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SRR4528A-3R3Y")</f>
+        <v>http://www.octopart.com/search?q=SRR4528A-3R3Y</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,18 +2585,18 @@
       <c r="F37" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G37" s="5" t="n">
-        <v>805</v>
+      <c r="G37" s="0" t="s">
+        <v>122</v>
       </c>
       <c r="H37" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LQW2BASR33J00L")</f>
-        <v>http://www.octopart.com/search?q=LQW2BASR33J00L</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=SRR4528A-2R2Y")</f>
+        <v>http://www.octopart.com/search?q=SRR4528A-2R2Y</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,18 +2618,18 @@
       <c r="F38" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>90</v>
+      <c r="G38" s="0" t="n">
+        <v>805</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J38" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=DMP3099L-7")</f>
-        <v>http://www.octopart.com/search?q=DMP3099L-7</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LQW2BASR24J00L")</f>
+        <v>http://www.octopart.com/search?q=LQW2BASR24J00L</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,22 +2651,18 @@
       <c r="F39" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>90</v>
+      <c r="G39" s="0" t="n">
+        <v>805</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J39" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=NUD3124LT1G")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=NUD3124LT1G</v>
-      </c>
-      <c r="K39" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=NUD3124LT1G")</f>
-        <v>http://www.octopart.com/search?q=NUD3124LT1G</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LQW2BASR27J00L")</f>
+        <v>http://www.octopart.com/search?q=LQW2BASR27J00L</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,18 +2684,18 @@
       <c r="F40" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>135</v>
+      <c r="G40" s="0" t="n">
+        <v>805</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J40" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AFT05MS003NT1")</f>
-        <v>http://www.octopart.com/search?q=AFT05MS003NT1</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LQW2BASR33J00L")</f>
+        <v>http://www.octopart.com/search?q=LQW2BASR33J00L</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,19 +2706,19 @@
         <v>17</v>
       </c>
       <c r="C41" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>137</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>90</v>
+        <v>137</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>3</v>
@@ -2699,94 +2727,86 @@
         <v>1</v>
       </c>
       <c r="J41" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MCP9700T-E/TT")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=MCP9700T-E/TT</v>
-      </c>
-      <c r="K41" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MCP9700T-E/TT")</f>
-        <v>http://www.octopart.com/search?q=MCP9700T-E/TT</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=DMP3099L-7")</f>
+        <v>http://www.octopart.com/search?q=DMP3099L-7</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>23867</v>
+      <c r="B42" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="C42" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="E42" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G42" s="5" t="n">
-        <v>603</v>
+      <c r="G42" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J42" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0733RL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0733RL</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=NUD3124LT1G")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=NUD3124LT1G</v>
       </c>
       <c r="K42" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-33R0ELF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-FX-33R0ELF</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=NUD3124LT1G")</f>
+        <v>http://www.octopart.com/search?q=NUD3124LT1G</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="0" t="n">
-        <v>26547</v>
+      <c r="B43" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="C43" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="E43" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="E43" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="5" t="n">
-        <v>603</v>
-      </c>
       <c r="H43" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="J43" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0710KL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0710KL</v>
-      </c>
-      <c r="K43" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1002HLF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-FX-1002HLF</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AFT05MS003NT1")</f>
+        <v>http://www.octopart.com/search?q=AFT05MS003NT1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>23666</v>
+      <c r="B44" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>145</v>
@@ -2795,126 +2815,134 @@
         <v>146</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="G44" s="5" t="n">
+      <c r="G44" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MCP9700T-E/TT")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=MCP9700T-E/TT</v>
+      </c>
+      <c r="K44" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MCP9700T-E/TT")</f>
+        <v>http://www.octopart.com/search?q=MCP9700T-E/TT</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>23867</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G45" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J44" s="0" t="str">
+      <c r="H45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J45" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0733RL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0733RL</v>
+      </c>
+      <c r="K45" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-33R0ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-33R0ELF</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>26547</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="J46" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0710KL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0710KL</v>
+      </c>
+      <c r="K46" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1002HLF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-1002HLF</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>23666</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-072R2L")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-072R2L</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="G45" s="5" t="n">
-        <v>603</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J45" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0735K7L")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0735K7L</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G46" s="5" t="n">
-        <v>603</v>
-      </c>
-      <c r="H46" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J46" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0711K5L")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0711K5L</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>4591</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="G47" s="5" t="n">
-        <v>603</v>
-      </c>
-      <c r="H47" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0720KL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0720KL</v>
-      </c>
-      <c r="K47" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-2002ELF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-FX-2002ELF</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2936,7 +2964,7 @@
       <c r="F48" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G48" s="5" t="n">
+      <c r="G48" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H48" s="0" t="n">
@@ -2946,16 +2974,16 @@
         <v>1</v>
       </c>
       <c r="J48" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0716K2L")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0716K2L</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0735K7L")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0735K7L</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="0" t="n">
-        <v>4597</v>
+      <c r="B49" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>160</v>
@@ -2966,34 +2994,34 @@
       <c r="E49" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F49" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="G49" s="5" t="n">
+      <c r="G49" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J49" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-072K2L")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-072K2L</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0711K5L")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0711K5L</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="0" t="s">
-        <v>17</v>
+      <c r="B50" s="0" t="n">
+        <v>4591</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="3" t="s">
         <v>164</v>
       </c>
       <c r="E50" s="0" t="s">
@@ -3002,7 +3030,7 @@
       <c r="F50" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="G50" s="5" t="n">
+      <c r="G50" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H50" s="0" t="n">
@@ -3012,8 +3040,12 @@
         <v>1</v>
       </c>
       <c r="J50" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0712K1L")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0712K1L</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0720KL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0720KL</v>
+      </c>
+      <c r="K50" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-2002ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-2002ELF</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,7 +3067,7 @@
       <c r="F51" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="G51" s="5" t="n">
+      <c r="G51" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H51" s="0" t="n">
@@ -3045,226 +3077,218 @@
         <v>1</v>
       </c>
       <c r="J51" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0716K2L")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0716K2L</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>4597</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J52" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-072K2L")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-072K2L</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0712K1L")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0712K1L</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07130RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-07130RL</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="B52" s="0" t="n">
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="0" t="n">
         <v>4682</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="G52" s="5" t="n">
+      <c r="C55" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="G55" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H52" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J52" s="0" t="str">
+      <c r="H55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0775RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0775RL</v>
       </c>
-      <c r="K52" s="0" t="str">
+      <c r="K55" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-75R0ELF")</f>
         <v>http://www.octopart.com/search?q=CR0603-FX-75R0ELF</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" s="0" t="n">
+    <row r="56" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="0" t="n">
         <v>23889</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E53" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="G53" s="5" t="n">
+      <c r="C56" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G56" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H53" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I53" s="0" t="n">
+      <c r="H56" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I56" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="J53" s="0" t="str">
+      <c r="J56" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-074K7L")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-074K7L</v>
       </c>
-      <c r="K53" s="0" t="str">
+      <c r="K56" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-4701ELF")</f>
         <v>http://www.octopart.com/search?q=CR0603-FX-4701ELF</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" s="0" t="n">
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="0" t="n">
         <v>4584</v>
       </c>
-      <c r="C54" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="G54" s="5" t="n">
+      <c r="C57" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H54" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J54" s="0" t="str">
+      <c r="H57" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-071K8L")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-071K8L</v>
       </c>
-      <c r="K54" s="0" t="str">
+      <c r="K57" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1801ELF")</f>
         <v>http://www.octopart.com/search?q=CR0603-FX-1801ELF</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>23987</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="G55" s="5" t="n">
-        <v>603</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I55" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J55" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-079K1L")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-079K1L</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>24078</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="G56" s="5" t="n">
-        <v>603</v>
-      </c>
-      <c r="H56" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I56" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J56" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0722RL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-0722RL</v>
-      </c>
-      <c r="K56" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-22R0ELF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-FX-22R0ELF</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G57" s="5" t="n">
-        <v>805</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I57" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J57" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0805FR-0712RL")</f>
-        <v>http://www.octopart.com/search?q=RC0805FR-0712RL</v>
-      </c>
-      <c r="K57" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ERJ-6ENF12R0V")</f>
-        <v>http://www.octopart.com/search?q=ERJ-6ENF12R0V</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3272,7 +3296,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>23514</v>
+        <v>23987</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>187</v>
@@ -3286,31 +3310,31 @@
       <c r="F58" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="G58" s="5" t="n">
+      <c r="G58" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I58" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J58" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07120RL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-07120RL</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-079K1L")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-079K1L</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>23865</v>
+        <v>24078</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>191</v>
       </c>
       <c r="E59" s="0" t="s">
@@ -3319,7 +3343,7 @@
       <c r="F59" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="G59" s="5" t="n">
+      <c r="G59" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H59" s="0" t="n">
@@ -3329,57 +3353,57 @@
         <v>2</v>
       </c>
       <c r="J59" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07330RL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-07330RL</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0722RL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-0722RL</v>
       </c>
       <c r="K59" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-3300ELF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-FX-3300ELF</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-22R0ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-22R0ELF</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="0" t="n">
-        <v>21904</v>
+      <c r="B60" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="3" t="s">
         <v>194</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F60" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G60" s="5" t="n">
-        <v>603</v>
+      <c r="G60" s="0" t="n">
+        <v>805</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I60" s="0" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J60" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-071KL")</f>
-        <v>http://www.octopart.com/search?q=RC0603FR-071KL</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0805FR-0712RL")</f>
+        <v>http://www.octopart.com/search?q=RC0805FR-0712RL</v>
       </c>
       <c r="K60" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1001HLF")</f>
-        <v>http://www.octopart.com/search?q=CR0603-FX-1001HLF</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ERJ-6ENF12R0V")</f>
+        <v>http://www.octopart.com/search?q=ERJ-6ENF12R0V</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="0" t="s">
-        <v>17</v>
+      <c r="B61" s="0" t="n">
+        <v>23514</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>196</v>
@@ -3393,363 +3417,355 @@
       <c r="F61" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="G61" s="5" t="n">
+      <c r="G61" s="0" t="n">
         <v>603</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I61" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J61" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07120RL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-07120RL</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>23865</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07330RL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-07330RL</v>
+      </c>
+      <c r="K62" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-3300ELF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-3300ELF</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>21904</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J63" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-071KL")</f>
+        <v>http://www.octopart.com/search?q=RC0603FR-071KL</v>
+      </c>
+      <c r="K63" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1001HLF")</f>
+        <v>http://www.octopart.com/search?q=CR0603-FX-1001HLF</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J64" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-071K6L")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-071K6L</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="B62" s="0" t="n">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="0" t="n">
         <v>23694</v>
       </c>
-      <c r="C62" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="G62" s="5" t="n">
+      <c r="C65" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="G65" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H62" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I62" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J62" s="0" t="str">
+      <c r="H65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J65" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-0727KL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-0727KL</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="B63" s="0" t="n">
+    <row r="66" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="0" t="n">
         <v>23502</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G63" s="5" t="n">
+      <c r="C66" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="G66" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H63" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I63" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J63" s="0" t="str">
+      <c r="H66" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J66" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07100RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-07100RL</v>
       </c>
-      <c r="K63" s="0" t="str">
+      <c r="K66" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-1000ELF")</f>
         <v>http://www.octopart.com/search?q=CR0603-FX-1000ELF</v>
       </c>
-      <c r="L63" s="0" t="str">
+      <c r="L66" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AC0603FR-07100RL")</f>
         <v>http://www.octopart.com/search?q=AC0603FR-07100RL</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="B64" s="0" t="n">
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="0" t="n">
         <v>23693</v>
       </c>
-      <c r="C64" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G64" s="5" t="n">
+      <c r="C67" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G67" s="0" t="n">
         <v>603</v>
       </c>
-      <c r="H64" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I64" s="0" t="n">
+      <c r="H67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I67" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="J64" s="0" t="str">
+      <c r="J67" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RC0603FR-07270RL")</f>
         <v>http://www.octopart.com/search?q=RC0603FR-07270RL</v>
       </c>
-      <c r="K64" s="0" t="str">
+      <c r="K67" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=CR0603-FX-2700ELF")</f>
         <v>http://www.octopart.com/search?q=CR0603-FX-2700ELF</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F65" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="G65" s="5" t="n">
+    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="G68" s="0" t="n">
         <v>1206</v>
       </c>
-      <c r="H65" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" s="0" t="str">
+      <c r="H68" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=RL1206FR-070R04L")</f>
         <v>http://www.octopart.com/search?q=RL1206FR-070R04L</v>
       </c>
-      <c r="K65" s="0" t="str">
+      <c r="K68" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PE1206FRM070R04L")</f>
         <v>http://www.octopart.com/search?q=PE1206FRM070R04L</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="E66" s="0" t="s">
+    <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E69" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F66" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H66" s="0" t="n">
+      <c r="F69" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="H69" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" s="0" t="str">
+      <c r="I69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=MABAES0060")</f>
         <v>http://www.aliexpress.com/wholesale?SearchText=MABAES0060</v>
       </c>
-      <c r="K66" s="0" t="str">
+      <c r="K69" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MABAES0060")</f>
         <v>http://www.octopart.com/search?q=MABAES0060</v>
       </c>
-      <c r="L66" s="0" t="str">
+      <c r="L69" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PWB1010-1LB")</f>
         <v>http://www.octopart.com/search?q=PWB1010-1LB</v>
       </c>
-      <c r="M66" s="0" t="str">
+      <c r="M69" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TC1-1TG2+")</f>
         <v>http://www.octopart.com/search?q=TC1-1TG2+</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>66</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E67" s="0" t="s">
+    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E70" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F67" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H67" s="0" t="n">
+      <c r="F70" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="H70" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J67" s="0" t="str">
+      <c r="I70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MABA-010143-FLUX18")</f>
         <v>http://www.octopart.com/search?q=MABA-010143-FLUX18</v>
       </c>
-      <c r="K67" s="0" t="str">
+      <c r="K70" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=WBC8-1LB")</f>
         <v>http://www.octopart.com/search?q=WBC8-1LB</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <v>67</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H68" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="I68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=B62152A4X30")</f>
-        <v>http://www.octopart.com/search?q=B62152A4X30</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>68</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H69" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="I69" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=S25FL116K0XMFI041")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=S25FL116K0XMFI041</v>
-      </c>
-      <c r="K69" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=W25Q16JVSNIQ")</f>
-        <v>http://www.octopart.com/search?q=W25Q16JVSNIQ</v>
-      </c>
-      <c r="L69" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=S25FL116K0XMFI043")</f>
-        <v>http://www.octopart.com/search?q=S25FL116K0XMFI043</v>
-      </c>
-      <c r="M69" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=S25FL116K0XMFI041")</f>
-        <v>http://www.octopart.com/search?q=S25FL116K0XMFI041</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <v>69</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>144</v>
-      </c>
-      <c r="I70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J70" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EP4CE22E22C8N")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=EP4CE22E22C8N</v>
-      </c>
-      <c r="K70" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EP4CE22E22C8N")</f>
-        <v>http://www.octopart.com/search?q=EP4CE22E22C8N</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3760,36 +3776,32 @@
         <v>17</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I71" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J71" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=st1s10")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=st1s10</v>
-      </c>
-      <c r="K71" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ST1S10PHR")</f>
-        <v>http://www.octopart.com/search?q=ST1S10PHR</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=B62152A4X30")</f>
+        <v>http://www.octopart.com/search?q=B62152A4X30</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
@@ -3797,37 +3809,41 @@
         <v>17</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="E72" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>233</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="I72" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J72" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=KSZ9031")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=KSZ9031</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=S25FL116K0XMFI041")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=S25FL116K0XMFI041</v>
       </c>
       <c r="K72" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=KSZ9031RNXCC")</f>
-        <v>http://www.octopart.com/search?q=KSZ9031RNXCC</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=W25Q16JVSNIQ")</f>
+        <v>http://www.octopart.com/search?q=W25Q16JVSNIQ</v>
       </c>
       <c r="L72" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=KSZ9031RNXCA")</f>
-        <v>http://www.octopart.com/search?q=KSZ9031RNXCA</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=S25FL116K0XMFI043")</f>
+        <v>http://www.octopart.com/search?q=S25FL116K0XMFI043</v>
+      </c>
+      <c r="M72" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=S25FL116K0XMFI041")</f>
+        <v>http://www.octopart.com/search?q=S25FL116K0XMFI041</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3838,29 +3854,33 @@
         <v>17</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E73" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>237</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="I73" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J73" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=5P49V5923B000NLGI")</f>
-        <v>http://www.octopart.com/search?q=5P49V5923B000NLGI</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=EP4CE22E22C8N")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=EP4CE22E22C8N</v>
+      </c>
+      <c r="K73" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=EP4CE22E22C8N")</f>
+        <v>http://www.octopart.com/search?q=EP4CE22E22C8N</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3871,36 +3891,36 @@
         <v>17</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E74" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>241</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="I74" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J74" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=AD9866BCPZ")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=AD9866BCPZ</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=st1s10")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=st1s10</v>
       </c>
       <c r="K74" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AD9866BCPZ")</f>
-        <v>http://www.octopart.com/search?q=AD9866BCPZ</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ST1S10PHR")</f>
+        <v>http://www.octopart.com/search?q=ST1S10PHR</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
@@ -3908,36 +3928,40 @@
         <v>17</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>246</v>
+        <v>242</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="E75" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>232</v>
+        <v>244</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="H75" s="0" t="n">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="I75" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J75" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=OPA2677")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=OPA2677</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=KSZ9031")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=KSZ9031</v>
       </c>
       <c r="K75" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=OPA2677IDDA")</f>
-        <v>http://www.octopart.com/search?q=OPA2677IDDA</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=KSZ9031RNXCC")</f>
+        <v>http://www.octopart.com/search?q=KSZ9031RNXCC</v>
+      </c>
+      <c r="L75" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=KSZ9031RNXCA")</f>
+        <v>http://www.octopart.com/search?q=KSZ9031RNXCA</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
@@ -3945,41 +3969,29 @@
         <v>17</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>247</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>249</v>
       </c>
       <c r="H76" s="0" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="I76" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J76" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=pe4259")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=pe4259</v>
-      </c>
-      <c r="K76" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=4259-63")</f>
-        <v>http://www.octopart.com/search?q=4259-63</v>
-      </c>
-      <c r="L76" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=4239-52")</f>
-        <v>http://www.octopart.com/search?q=4239-52</v>
-      </c>
-      <c r="M76" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PE42421SCAA")</f>
-        <v>http://www.octopart.com/search?q=PE42421SCAA</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=5P49V5923B000NLGI")</f>
+        <v>http://www.octopart.com/search?q=5P49V5923B000NLGI</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3990,29 +4002,33 @@
         <v>17</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>232</v>
+        <v>252</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>253</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="I77" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J77" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AP2204MP-ADJTRG1")</f>
-        <v>http://www.octopart.com/search?q=AP2204MP-ADJTRG1</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=AD9866BCPZ")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=AD9866BCPZ</v>
+      </c>
+      <c r="K77" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AD9866BCPZ")</f>
+        <v>http://www.octopart.com/search?q=AD9866BCPZ</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4023,19 +4039,19 @@
         <v>17</v>
       </c>
       <c r="C78" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="D78" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>256</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>241</v>
       </c>
       <c r="H78" s="0" t="n">
         <v>8</v>
@@ -4044,11 +4060,15 @@
         <v>1</v>
       </c>
       <c r="J78" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MAX11613EUA")</f>
-        <v>http://www.octopart.com/search?q=MAX11613EUA</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=OPA2677")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=OPA2677</v>
+      </c>
+      <c r="K78" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=OPA2677IDDA")</f>
+        <v>http://www.octopart.com/search?q=OPA2677IDDA</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
@@ -4056,29 +4076,41 @@
         <v>17</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>260</v>
+        <v>257</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="E79" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>260</v>
       </c>
       <c r="H79" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I79" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J79" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=INA199A1DCKR")</f>
-        <v>http://www.octopart.com/search?q=INA199A1DCKR</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=pe4259")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=pe4259</v>
+      </c>
+      <c r="K79" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=4259-63")</f>
+        <v>http://www.octopart.com/search?q=4259-63</v>
+      </c>
+      <c r="L79" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=4239-52")</f>
+        <v>http://www.octopart.com/search?q=4239-52</v>
+      </c>
+      <c r="M79" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=PE42421SCAA")</f>
+        <v>http://www.octopart.com/search?q=PE42421SCAA</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4089,29 +4121,29 @@
         <v>17</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E80" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>241</v>
       </c>
       <c r="H80" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I80" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J80" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MCP4662-502E/UN")</f>
-        <v>http://www.octopart.com/search?q=MCP4662-502E/UN</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=AP2204MP-ADJTRG1")</f>
+        <v>http://www.octopart.com/search?q=AP2204MP-ADJTRG1</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4122,33 +4154,29 @@
         <v>17</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>267</v>
       </c>
       <c r="H81" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I81" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J81" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=TPS73025DBVR")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=TPS73025DBVR</v>
-      </c>
-      <c r="K81" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TPS73025DBVR")</f>
-        <v>http://www.octopart.com/search?q=TPS73025DBVR</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MAX11613EUA")</f>
+        <v>http://www.octopart.com/search?q=MAX11613EUA</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4159,29 +4187,29 @@
         <v>17</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>271</v>
       </c>
       <c r="H82" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I82" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J82" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LP2985-10DBVR")</f>
-        <v>http://www.octopart.com/search?q=LP2985-10DBVR</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=INA199A1DCKR")</f>
+        <v>http://www.octopart.com/search?q=INA199A1DCKR</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4192,33 +4220,29 @@
         <v>17</v>
       </c>
       <c r="C83" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D83" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="E83" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="E83" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F83" s="0" t="s">
+      <c r="G83" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="G83" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="H83" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I83" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J83" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG</v>
-      </c>
-      <c r="K83" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=400R0111-24-9")</f>
-        <v>http://www.octopart.com/search?q=400R0111-24-9</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=MCP4662-502E/UN")</f>
+        <v>http://www.octopart.com/search?q=MCP4662-502E/UN</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,33 +4253,33 @@
         <v>17</v>
       </c>
       <c r="C84" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="D84" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="D84" s="0" t="s">
+      <c r="E84" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F84" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="E84" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F84" s="0" t="s">
+      <c r="G84" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="G84" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="H84" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I84" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J84" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=25mhz 3.2x2.5 passive")</f>
-        <v>http://www.aliexpress.com/wholesale?SearchText=25mhz 3.2x2.5 passive</v>
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=TPS73025DBVR")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=TPS73025DBVR</v>
       </c>
       <c r="K84" s="0" t="str">
-        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=NX3225SA-25.000M-STD-CSR-3")</f>
-        <v>http://www.octopart.com/search?q=NX3225SA-25.000M-STD-CSR-3</v>
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=TPS73025DBVR")</f>
+        <v>http://www.octopart.com/search?q=TPS73025DBVR</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,102 +4290,204 @@
         <v>17</v>
       </c>
       <c r="C85" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D85" s="0" t="s">
         <v>280</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>281</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F85" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=LP2985-10DBVR")</f>
+        <v>http://www.octopart.com/search?q=LP2985-10DBVR</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="G85" s="5" t="s">
+      <c r="D86" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="H85" s="0" t="n">
+      <c r="E86" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=PFTE Teflon Silver Plated Wire 30AWG</v>
+      </c>
+      <c r="K86" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=400R0111-24-9")</f>
+        <v>http://www.octopart.com/search?q=400R0111-24-9</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="H87" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I85" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" s="0" t="str">
+      <c r="I87" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.aliexpress.com/wholesale?SearchText=25mhz 3.2x2.5 passive")</f>
+        <v>http://www.aliexpress.com/wholesale?SearchText=25mhz 3.2x2.5 passive</v>
+      </c>
+      <c r="K87" s="0" t="str">
+        <f aca="false">HYPERLINK("http://www.octopart.com/search?q=NX3225SA-25.000M-STD-CSR-3")</f>
+        <v>http://www.octopart.com/search?q=NX3225SA-25.000M-STD-CSR-3</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="H88" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" s="0" t="str">
         <f aca="false">HYPERLINK("http://www.octopart.com/search?q=ASTXR-12-38.400MHZ-514054-T")</f>
         <v>http://www.octopart.com/search?q=ASTXR-12-38.400MHZ-514054-T</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G86" s="5"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B87" s="0" t="n">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B90" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="D87" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G87" s="5"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="B88" s="0" t="n">
-        <v>368</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="D88" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G88" s="5"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="B89" s="0" t="n">
-        <v>1093</v>
-      </c>
-      <c r="C89" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="D89" s="0" t="n">
+      <c r="C90" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>1097</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D92" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="G89" s="5"/>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G90" s="5"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B91" s="1"/>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+    </row>
+    <row r="95" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="J1:N1"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A95:D95"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>